<commit_message>
Update the transition matrix
</commit_message>
<xml_diff>
--- a/03_Output/02_Tables/Transition-of-Heating-Type.xlsx
+++ b/03_Output/02_Tables/Transition-of-Heating-Type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmjo/Dropbox/00_JMJo/Projects/CER-Trial/03_Output/02_Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62413F5-E57F-9348-ABBF-B80CBD96E880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF01C226-2B0B-394A-8AEE-5F28CD113683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34140" windowHeight="28300" xr2:uid="{B70FB47A-1447-D048-A83B-2A87D7E8B32A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="20">
   <si>
     <t>T</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -94,6 +94,26 @@
   </si>
   <si>
     <t>Unknown for Space &amp; Unknown for Water in Pre-Survey</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unknown for Space &amp; Electric for Water in Pre-Survey</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unknown for Space &amp; Non-Electric for Water in Pre-Survey</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electric for Space &amp; Unknown for Water in Pre-Survey</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-Electric for Space &amp; Unknown for Water in Pre-Survey</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summary</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -371,7 +391,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -457,6 +477,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -773,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{743A5A0E-51FE-9B43-B0B4-7FA6EAD9C3B1}">
-  <dimension ref="B1:AG42"/>
+  <dimension ref="B1:AG83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="W38" sqref="W38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="AC81" sqref="AC81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -2264,13 +2302,1511 @@
       <c r="AF40" s="28"/>
       <c r="AG40" s="28"/>
     </row>
-    <row r="41" spans="2:33" ht="10" customHeight="1">
+    <row r="41" spans="2:33" ht="20" customHeight="1">
       <c r="AF41" s="28"/>
       <c r="AG41" s="28"/>
     </row>
-    <row r="42" spans="2:33" ht="10" customHeight="1">
+    <row r="42" spans="2:33" ht="25" customHeight="1">
+      <c r="B42" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="Z42" s="1"/>
       <c r="AF42" s="28"/>
       <c r="AG42" s="28"/>
+    </row>
+    <row r="43" spans="2:33" ht="25" customHeight="1">
+      <c r="B43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF43" s="28"/>
+      <c r="AG43" s="28"/>
+    </row>
+    <row r="44" spans="2:33" ht="30" customHeight="1">
+      <c r="D44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="4"/>
+      <c r="J44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K44" s="3"/>
+      <c r="L44" s="4"/>
+      <c r="P44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="4"/>
+      <c r="V44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W44" s="3"/>
+      <c r="X44" s="4"/>
+      <c r="AB44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC44" s="3"/>
+      <c r="AD44" s="4"/>
+      <c r="AF44" s="28"/>
+      <c r="AG44" s="28"/>
+    </row>
+    <row r="45" spans="2:33" ht="30" customHeight="1">
+      <c r="D45" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L45" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P45" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R45" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="V45" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W45" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="X45" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB45" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD45" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF45" s="28"/>
+      <c r="AG45" s="28"/>
+    </row>
+    <row r="46" spans="2:33" ht="40" customHeight="1">
+      <c r="B46" s="5"/>
+      <c r="C46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="13"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="15">
+        <v>39</v>
+      </c>
+      <c r="H46" s="5"/>
+      <c r="I46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J46" s="13"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="15"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P46" s="13">
+        <v>3</v>
+      </c>
+      <c r="Q46" s="14">
+        <v>9</v>
+      </c>
+      <c r="R46" s="15">
+        <f xml:space="preserve"> SUM(P46:Q48, R47:R48) * -1</f>
+        <v>-39</v>
+      </c>
+      <c r="T46" s="5"/>
+      <c r="U46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="V46" s="13"/>
+      <c r="W46" s="14"/>
+      <c r="X46" s="15"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="13">
+        <f xml:space="preserve"> SUM(D46, P46, V46)</f>
+        <v>3</v>
+      </c>
+      <c r="AC46" s="14">
+        <f t="shared" ref="AC46:AC48" si="15" xml:space="preserve"> SUM(E46, Q46, W46)</f>
+        <v>9</v>
+      </c>
+      <c r="AD46" s="30">
+        <f t="shared" ref="AD46:AD48" si="16" xml:space="preserve"> SUM(F46, R46, X46)</f>
+        <v>0</v>
+      </c>
+      <c r="AF46" s="28"/>
+      <c r="AG46" s="28"/>
+    </row>
+    <row r="47" spans="2:33" ht="40" customHeight="1">
+      <c r="B47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="16"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="18"/>
+      <c r="H47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47" s="16"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="18"/>
+      <c r="N47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O47" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P47" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q47" s="17">
+        <v>18</v>
+      </c>
+      <c r="R47" s="18"/>
+      <c r="T47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U47" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="V47" s="16"/>
+      <c r="W47" s="17"/>
+      <c r="X47" s="18"/>
+      <c r="Z47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA47" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB47" s="16">
+        <f t="shared" ref="AB47:AB48" si="17" xml:space="preserve"> SUM(D47, P47, V47)</f>
+        <v>3</v>
+      </c>
+      <c r="AC47" s="17">
+        <f t="shared" si="15"/>
+        <v>18</v>
+      </c>
+      <c r="AD47" s="18">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AF47" s="28"/>
+      <c r="AG47" s="28"/>
+    </row>
+    <row r="48" spans="2:33" ht="40" customHeight="1">
+      <c r="B48" s="7"/>
+      <c r="C48" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="19"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="21"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J48" s="19"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="21"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="21">
+        <v>6</v>
+      </c>
+      <c r="T48" s="7"/>
+      <c r="U48" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="V48" s="19"/>
+      <c r="W48" s="20"/>
+      <c r="X48" s="21"/>
+      <c r="Z48" s="7"/>
+      <c r="AA48" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB48" s="19">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AC48" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD48" s="29">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="AF48" s="28"/>
+      <c r="AG48" s="28"/>
+    </row>
+    <row r="49" spans="2:33" ht="20" customHeight="1">
+      <c r="AF49" s="28"/>
+      <c r="AG49" s="28"/>
+    </row>
+    <row r="50" spans="2:33" ht="25" customHeight="1">
+      <c r="B50" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AF50" s="28"/>
+      <c r="AG50" s="28"/>
+    </row>
+    <row r="51" spans="2:33" ht="25" customHeight="1">
+      <c r="B51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF51" s="28"/>
+      <c r="AG51" s="28"/>
+    </row>
+    <row r="52" spans="2:33" ht="30" customHeight="1">
+      <c r="D52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="4"/>
+      <c r="J52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K52" s="3"/>
+      <c r="L52" s="4"/>
+      <c r="P52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="4"/>
+      <c r="V52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W52" s="3"/>
+      <c r="X52" s="4"/>
+      <c r="AB52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC52" s="3"/>
+      <c r="AD52" s="4"/>
+      <c r="AF52" s="28"/>
+      <c r="AG52" s="28"/>
+    </row>
+    <row r="53" spans="2:33" ht="30" customHeight="1">
+      <c r="D53" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K53" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L53" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P53" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R53" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="V53" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W53" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="X53" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB53" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD53" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF53" s="28"/>
+      <c r="AG53" s="28"/>
+    </row>
+    <row r="54" spans="2:33" ht="40" customHeight="1">
+      <c r="B54" s="5"/>
+      <c r="C54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="13"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="15"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J54" s="13"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="15"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="14">
+        <v>3</v>
+      </c>
+      <c r="R54" s="15"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="V54" s="13"/>
+      <c r="W54" s="14"/>
+      <c r="X54" s="15"/>
+      <c r="Z54" s="5"/>
+      <c r="AA54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB54" s="13">
+        <f xml:space="preserve"> SUM(D54, P54, V54)</f>
+        <v>0</v>
+      </c>
+      <c r="AC54" s="14">
+        <f t="shared" ref="AC54:AC56" si="18" xml:space="preserve"> SUM(E54, Q54, W54)</f>
+        <v>3</v>
+      </c>
+      <c r="AD54" s="15">
+        <f t="shared" ref="AD54:AD56" si="19" xml:space="preserve"> SUM(F54, R54, X54)</f>
+        <v>0</v>
+      </c>
+      <c r="AF54" s="28"/>
+      <c r="AG54" s="28"/>
+    </row>
+    <row r="55" spans="2:33" ht="40" customHeight="1">
+      <c r="B55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" s="16"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="18">
+        <v>49</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J55" s="16"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="18"/>
+      <c r="N55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O55" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P55" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="17">
+        <v>38</v>
+      </c>
+      <c r="R55" s="18">
+        <f xml:space="preserve"> SUM(P54:Q56, R54, R56) * -1</f>
+        <v>-49</v>
+      </c>
+      <c r="T55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U55" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="V55" s="16"/>
+      <c r="W55" s="17"/>
+      <c r="X55" s="18"/>
+      <c r="Z55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA55" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB55" s="16">
+        <f t="shared" ref="AB55:AB56" si="20" xml:space="preserve"> SUM(D55, P55, V55)</f>
+        <v>1</v>
+      </c>
+      <c r="AC55" s="17">
+        <f t="shared" si="18"/>
+        <v>38</v>
+      </c>
+      <c r="AD55" s="31">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AF55" s="28"/>
+      <c r="AG55" s="28"/>
+    </row>
+    <row r="56" spans="2:33" ht="40" customHeight="1">
+      <c r="B56" s="7"/>
+      <c r="C56" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="19"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="21"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J56" s="19"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="21"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P56" s="19"/>
+      <c r="Q56" s="20"/>
+      <c r="R56" s="21">
+        <v>7</v>
+      </c>
+      <c r="T56" s="7"/>
+      <c r="U56" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="V56" s="19"/>
+      <c r="W56" s="20"/>
+      <c r="X56" s="21"/>
+      <c r="Z56" s="7"/>
+      <c r="AA56" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB56" s="19">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AC56" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AD56" s="29">
+        <f t="shared" si="19"/>
+        <v>7</v>
+      </c>
+      <c r="AF56" s="28"/>
+      <c r="AG56" s="28"/>
+    </row>
+    <row r="57" spans="2:33" ht="20" customHeight="1">
+      <c r="AF57" s="28"/>
+      <c r="AG57" s="28"/>
+    </row>
+    <row r="58" spans="2:33" ht="25" customHeight="1">
+      <c r="B58" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="Z58" s="1"/>
+      <c r="AF58" s="28"/>
+      <c r="AG58" s="28"/>
+    </row>
+    <row r="59" spans="2:33" ht="25" customHeight="1">
+      <c r="B59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF59" s="28"/>
+      <c r="AG59" s="28"/>
+    </row>
+    <row r="60" spans="2:33" ht="30" customHeight="1">
+      <c r="D60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="3"/>
+      <c r="F60" s="4"/>
+      <c r="J60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K60" s="3"/>
+      <c r="L60" s="4"/>
+      <c r="P60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="4"/>
+      <c r="V60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W60" s="3"/>
+      <c r="X60" s="4"/>
+      <c r="AB60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC60" s="3"/>
+      <c r="AD60" s="4"/>
+      <c r="AF60" s="28"/>
+      <c r="AG60" s="28"/>
+    </row>
+    <row r="61" spans="2:33" ht="30" customHeight="1">
+      <c r="D61" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J61" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K61" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L61" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P61" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R61" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="V61" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W61" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="X61" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB61" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC61" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD61" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF61" s="28"/>
+      <c r="AG61" s="28"/>
+    </row>
+    <row r="62" spans="2:33" ht="40" customHeight="1">
+      <c r="B62" s="5"/>
+      <c r="C62" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="13"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="15"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J62" s="13"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="15"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P62" s="13"/>
+      <c r="Q62" s="14">
+        <v>3</v>
+      </c>
+      <c r="R62" s="15"/>
+      <c r="T62" s="5"/>
+      <c r="U62" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="V62" s="13"/>
+      <c r="W62" s="14"/>
+      <c r="X62" s="15"/>
+      <c r="Z62" s="5"/>
+      <c r="AA62" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="13">
+        <f xml:space="preserve"> SUM(D62, P62, V62)</f>
+        <v>0</v>
+      </c>
+      <c r="AC62" s="14">
+        <f t="shared" ref="AC62:AC64" si="21" xml:space="preserve"> SUM(E62, Q62, W62)</f>
+        <v>3</v>
+      </c>
+      <c r="AD62" s="15">
+        <f t="shared" ref="AD62:AD64" si="22" xml:space="preserve"> SUM(F62, R62, X62)</f>
+        <v>0</v>
+      </c>
+      <c r="AF62" s="28"/>
+      <c r="AG62" s="28"/>
+    </row>
+    <row r="63" spans="2:33" ht="40" customHeight="1">
+      <c r="B63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="16"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="18"/>
+      <c r="H63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J63" s="16"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="18"/>
+      <c r="N63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O63" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P63" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="17">
+        <v>9</v>
+      </c>
+      <c r="R63" s="18"/>
+      <c r="T63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U63" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="V63" s="16"/>
+      <c r="W63" s="17"/>
+      <c r="X63" s="18"/>
+      <c r="Z63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA63" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB63" s="16">
+        <f t="shared" ref="AB63" si="23" xml:space="preserve"> SUM(D63, P63, V63)</f>
+        <v>1</v>
+      </c>
+      <c r="AC63" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="AD63" s="18">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF63" s="28"/>
+      <c r="AG63" s="28"/>
+    </row>
+    <row r="64" spans="2:33" ht="40" customHeight="1">
+      <c r="B64" s="7"/>
+      <c r="C64" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="19">
+        <v>15</v>
+      </c>
+      <c r="E64" s="20"/>
+      <c r="F64" s="21"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J64" s="19"/>
+      <c r="K64" s="20"/>
+      <c r="L64" s="21"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P64" s="19">
+        <f xml:space="preserve"> SUM(P62:R63, Q64:R64) * -1</f>
+        <v>-15</v>
+      </c>
+      <c r="Q64" s="20"/>
+      <c r="R64" s="21">
+        <v>2</v>
+      </c>
+      <c r="T64" s="7"/>
+      <c r="U64" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="V64" s="19"/>
+      <c r="W64" s="20"/>
+      <c r="X64" s="21"/>
+      <c r="Z64" s="7"/>
+      <c r="AA64" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB64" s="32">
+        <f xml:space="preserve"> SUM(D64, P64, V64)</f>
+        <v>0</v>
+      </c>
+      <c r="AC64" s="20">
+        <f xml:space="preserve"> SUM(E64, Q64, W64)</f>
+        <v>0</v>
+      </c>
+      <c r="AD64" s="29">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="AF64" s="28"/>
+      <c r="AG64" s="28"/>
+    </row>
+    <row r="65" spans="2:33" ht="20" customHeight="1">
+      <c r="AF65" s="28"/>
+      <c r="AG65" s="28"/>
+    </row>
+    <row r="66" spans="2:33" ht="25" customHeight="1">
+      <c r="B66" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="Z66" s="1"/>
+      <c r="AF66" s="28"/>
+      <c r="AG66" s="28"/>
+    </row>
+    <row r="67" spans="2:33" ht="25" customHeight="1">
+      <c r="B67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF67" s="28"/>
+      <c r="AG67" s="28"/>
+    </row>
+    <row r="68" spans="2:33" ht="30" customHeight="1">
+      <c r="D68" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="3"/>
+      <c r="F68" s="4"/>
+      <c r="J68" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K68" s="3"/>
+      <c r="L68" s="4"/>
+      <c r="P68" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="4"/>
+      <c r="V68" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W68" s="3"/>
+      <c r="X68" s="4"/>
+      <c r="AB68" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC68" s="3"/>
+      <c r="AD68" s="4"/>
+      <c r="AF68" s="28"/>
+      <c r="AG68" s="28"/>
+    </row>
+    <row r="69" spans="2:33" ht="30" customHeight="1">
+      <c r="D69" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K69" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L69" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P69" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R69" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="V69" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W69" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="X69" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB69" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC69" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD69" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF69" s="28"/>
+      <c r="AG69" s="28"/>
+    </row>
+    <row r="70" spans="2:33" ht="40" customHeight="1">
+      <c r="B70" s="5"/>
+      <c r="C70" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="13"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="15"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J70" s="13"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="15"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P70" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q70" s="14">
+        <v>88</v>
+      </c>
+      <c r="R70" s="15"/>
+      <c r="T70" s="5"/>
+      <c r="U70" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="V70" s="13"/>
+      <c r="W70" s="14"/>
+      <c r="X70" s="15"/>
+      <c r="Z70" s="5"/>
+      <c r="AA70" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB70" s="13">
+        <f xml:space="preserve"> SUM(D70, P70, V70)</f>
+        <v>8</v>
+      </c>
+      <c r="AC70" s="14">
+        <f t="shared" ref="AC70:AC72" si="24" xml:space="preserve"> SUM(E70, Q70, W70)</f>
+        <v>88</v>
+      </c>
+      <c r="AD70" s="15">
+        <f t="shared" ref="AD70:AD72" si="25" xml:space="preserve"> SUM(F70, R70, X70)</f>
+        <v>0</v>
+      </c>
+      <c r="AF70" s="28"/>
+      <c r="AG70" s="28"/>
+    </row>
+    <row r="71" spans="2:33" ht="40" customHeight="1">
+      <c r="B71" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" s="16"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="18"/>
+      <c r="H71" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I71" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J71" s="16"/>
+      <c r="K71" s="17"/>
+      <c r="L71" s="18"/>
+      <c r="N71" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O71" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P71" s="16">
+        <v>29</v>
+      </c>
+      <c r="Q71" s="17">
+        <v>1116</v>
+      </c>
+      <c r="R71" s="18"/>
+      <c r="T71" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U71" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="V71" s="16"/>
+      <c r="W71" s="17"/>
+      <c r="X71" s="18"/>
+      <c r="Z71" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA71" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB71" s="16">
+        <f t="shared" ref="AB71:AB72" si="26" xml:space="preserve"> SUM(D71, P71, V71)</f>
+        <v>29</v>
+      </c>
+      <c r="AC71" s="17">
+        <f t="shared" si="24"/>
+        <v>1116</v>
+      </c>
+      <c r="AD71" s="18">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AF71" s="28"/>
+      <c r="AG71" s="28"/>
+    </row>
+    <row r="72" spans="2:33" ht="40" customHeight="1">
+      <c r="B72" s="7"/>
+      <c r="C72" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="19"/>
+      <c r="E72" s="20">
+        <v>1383</v>
+      </c>
+      <c r="F72" s="21"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J72" s="19"/>
+      <c r="K72" s="20"/>
+      <c r="L72" s="21"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P72" s="19"/>
+      <c r="Q72" s="20">
+        <f xml:space="preserve"> SUM(P70:R71, P72, R72) * -1</f>
+        <v>-1383</v>
+      </c>
+      <c r="R72" s="21">
+        <v>142</v>
+      </c>
+      <c r="T72" s="7"/>
+      <c r="U72" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="V72" s="19"/>
+      <c r="W72" s="20"/>
+      <c r="X72" s="21"/>
+      <c r="Z72" s="7"/>
+      <c r="AA72" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB72" s="19">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="AC72" s="33">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AD72" s="29">
+        <f t="shared" si="25"/>
+        <v>142</v>
+      </c>
+      <c r="AF72" s="28"/>
+      <c r="AG72" s="28"/>
+    </row>
+    <row r="73" spans="2:33" ht="20" customHeight="1">
+      <c r="AF73" s="28"/>
+      <c r="AG73" s="28"/>
+    </row>
+    <row r="74" spans="2:33" ht="20" customHeight="1">
+      <c r="AF74" s="28"/>
+      <c r="AG74" s="28"/>
+    </row>
+    <row r="75" spans="2:33" ht="25" customHeight="1">
+      <c r="B75" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="Z75" s="1"/>
+      <c r="AF75" s="28"/>
+      <c r="AG75" s="28"/>
+    </row>
+    <row r="76" spans="2:33" ht="25" customHeight="1">
+      <c r="B76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF76" s="28"/>
+      <c r="AG76" s="28"/>
+    </row>
+    <row r="77" spans="2:33" ht="30" customHeight="1">
+      <c r="D77" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="3"/>
+      <c r="F77" s="4"/>
+      <c r="J77" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K77" s="3"/>
+      <c r="L77" s="4"/>
+      <c r="P77" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q77" s="3"/>
+      <c r="R77" s="4"/>
+      <c r="V77" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W77" s="3"/>
+      <c r="X77" s="4"/>
+      <c r="AB77" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC77" s="3"/>
+      <c r="AD77" s="4"/>
+      <c r="AF77" s="28"/>
+      <c r="AG77" s="28"/>
+    </row>
+    <row r="78" spans="2:33" ht="30" customHeight="1">
+      <c r="D78" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J78" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K78" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L78" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P78" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R78" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="V78" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W78" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="X78" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB78" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC78" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD78" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF78" s="28"/>
+      <c r="AG78" s="28"/>
+    </row>
+    <row r="79" spans="2:33" ht="40" customHeight="1">
+      <c r="B79" s="5"/>
+      <c r="C79" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="13">
+        <f xml:space="preserve"> SUM(D6,D14,D22,D30,D38,D46,D54,D62,D70)</f>
+        <v>29</v>
+      </c>
+      <c r="E79" s="14">
+        <f t="shared" ref="E79:F79" si="27" xml:space="preserve"> SUM(E6,E14,E22,E30,E38,E46,E54,E62,E70)</f>
+        <v>371</v>
+      </c>
+      <c r="F79" s="15">
+        <f t="shared" si="27"/>
+        <v>39</v>
+      </c>
+      <c r="H79" s="5"/>
+      <c r="I79" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J79" s="13">
+        <f xml:space="preserve"> SUM(J6,J14,J22,J30,J38,J46,J54,J62,J70)</f>
+        <v>7</v>
+      </c>
+      <c r="K79" s="14">
+        <f t="shared" ref="K79:L79" si="28" xml:space="preserve"> SUM(K6,K14,K22,K30,K38,K46,K54,K62,K70)</f>
+        <v>89</v>
+      </c>
+      <c r="L79" s="15">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="N79" s="5"/>
+      <c r="O79" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P79" s="13">
+        <f xml:space="preserve"> SUM(P6,P14,P22,P30,P38,P46,P54,P62,P70)</f>
+        <v>11</v>
+      </c>
+      <c r="Q79" s="14">
+        <f t="shared" ref="Q79:R79" si="29" xml:space="preserve"> SUM(Q6,Q14,Q22,Q30,Q38,Q46,Q54,Q62,Q70)</f>
+        <v>-91</v>
+      </c>
+      <c r="R79" s="15">
+        <f t="shared" si="29"/>
+        <v>-39</v>
+      </c>
+      <c r="T79" s="5"/>
+      <c r="U79" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="V79" s="13">
+        <f xml:space="preserve"> SUM(V6,V14,V22,V30,V38,V46,V54,V62,V70)</f>
+        <v>11</v>
+      </c>
+      <c r="W79" s="14">
+        <f t="shared" ref="W79:X79" si="30" xml:space="preserve"> SUM(W6,W14,W22,W30,W38,W46,W54,W62,W70)</f>
+        <v>-91</v>
+      </c>
+      <c r="X79" s="15">
+        <f t="shared" si="30"/>
+        <v>-39</v>
+      </c>
+      <c r="Z79" s="5"/>
+      <c r="AA79" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB79" s="13">
+        <f xml:space="preserve"> SUM(D79, P79, V79)</f>
+        <v>51</v>
+      </c>
+      <c r="AC79" s="14">
+        <f t="shared" ref="AC79:AC81" si="31" xml:space="preserve"> SUM(E79, Q79, W79)</f>
+        <v>189</v>
+      </c>
+      <c r="AD79" s="15">
+        <f t="shared" ref="AD79:AD81" si="32" xml:space="preserve"> SUM(F79, R79, X79)</f>
+        <v>-39</v>
+      </c>
+      <c r="AF79" s="28"/>
+      <c r="AG79" s="28"/>
+    </row>
+    <row r="80" spans="2:33" ht="40" customHeight="1">
+      <c r="B80" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80" s="16">
+        <f t="shared" ref="D80:F80" si="33" xml:space="preserve"> SUM(D7,D15,D23,D31,D39,D47,D55,D63,D71)</f>
+        <v>26</v>
+      </c>
+      <c r="E80" s="17">
+        <f t="shared" si="33"/>
+        <v>1380</v>
+      </c>
+      <c r="F80" s="18">
+        <f t="shared" si="33"/>
+        <v>49</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I80" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J80" s="16">
+        <f t="shared" ref="J80:L80" si="34" xml:space="preserve"> SUM(J7,J15,J23,J31,J39,J47,J55,J63,J71)</f>
+        <v>1</v>
+      </c>
+      <c r="K80" s="17">
+        <f t="shared" si="34"/>
+        <v>1170</v>
+      </c>
+      <c r="L80" s="18">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="N80" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O80" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P80" s="16">
+        <f t="shared" ref="P80:R80" si="35" xml:space="preserve"> SUM(P7,P15,P23,P31,P39,P47,P55,P63,P71)</f>
+        <v>54</v>
+      </c>
+      <c r="Q80" s="17">
+        <f t="shared" si="35"/>
+        <v>1524</v>
+      </c>
+      <c r="R80" s="18">
+        <f t="shared" si="35"/>
+        <v>-49</v>
+      </c>
+      <c r="T80" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U80" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="V80" s="16">
+        <f t="shared" ref="V80:X80" si="36" xml:space="preserve"> SUM(V7,V15,V23,V31,V39,V47,V55,V63,V71)</f>
+        <v>54</v>
+      </c>
+      <c r="W80" s="17">
+        <f t="shared" si="36"/>
+        <v>1524</v>
+      </c>
+      <c r="X80" s="18">
+        <f t="shared" si="36"/>
+        <v>-49</v>
+      </c>
+      <c r="Z80" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA80" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB80" s="16">
+        <f t="shared" ref="AB80:AB81" si="37" xml:space="preserve"> SUM(D80, P80, V80)</f>
+        <v>134</v>
+      </c>
+      <c r="AC80" s="17">
+        <f t="shared" si="31"/>
+        <v>4428</v>
+      </c>
+      <c r="AD80" s="18">
+        <f t="shared" si="32"/>
+        <v>-49</v>
+      </c>
+      <c r="AF80" s="28"/>
+      <c r="AG80" s="28"/>
+    </row>
+    <row r="81" spans="2:33" ht="40" customHeight="1">
+      <c r="B81" s="7"/>
+      <c r="C81" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="19">
+        <f t="shared" ref="D81:F81" si="38" xml:space="preserve"> SUM(D8,D16,D24,D32,D40,D48,D56,D64,D72)</f>
+        <v>15</v>
+      </c>
+      <c r="E81" s="20">
+        <f t="shared" si="38"/>
+        <v>1383</v>
+      </c>
+      <c r="F81" s="21">
+        <f t="shared" si="38"/>
+        <v>795</v>
+      </c>
+      <c r="H81" s="7"/>
+      <c r="I81" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J81" s="19">
+        <f t="shared" ref="J81:L81" si="39" xml:space="preserve"> SUM(J8,J16,J24,J32,J40,J48,J56,J64,J72)</f>
+        <v>0</v>
+      </c>
+      <c r="K81" s="20">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="L81" s="21">
+        <f t="shared" si="39"/>
+        <v>444</v>
+      </c>
+      <c r="N81" s="7"/>
+      <c r="O81" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P81" s="19">
+        <f t="shared" ref="P81:R81" si="40" xml:space="preserve"> SUM(P8,P16,P24,P32,P40,P48,P56,P64,P72)</f>
+        <v>-15</v>
+      </c>
+      <c r="Q81" s="20">
+        <f t="shared" si="40"/>
+        <v>-1383</v>
+      </c>
+      <c r="R81" s="21">
+        <f t="shared" si="40"/>
+        <v>-12</v>
+      </c>
+      <c r="T81" s="7"/>
+      <c r="U81" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="V81" s="19">
+        <f t="shared" ref="V81:X81" si="41" xml:space="preserve"> SUM(V8,V16,V24,V32,V40,V48,V56,V64,V72)</f>
+        <v>-15</v>
+      </c>
+      <c r="W81" s="20">
+        <f t="shared" si="41"/>
+        <v>-1383</v>
+      </c>
+      <c r="X81" s="21">
+        <f t="shared" si="41"/>
+        <v>-12</v>
+      </c>
+      <c r="Z81" s="7"/>
+      <c r="AA81" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB81" s="19">
+        <f t="shared" si="37"/>
+        <v>-15</v>
+      </c>
+      <c r="AC81" s="34">
+        <f t="shared" si="31"/>
+        <v>-1383</v>
+      </c>
+      <c r="AD81" s="29">
+        <f t="shared" si="32"/>
+        <v>771</v>
+      </c>
+      <c r="AF81" s="28"/>
+      <c r="AG81" s="28"/>
+    </row>
+    <row r="82" spans="2:33" ht="10" customHeight="1">
+      <c r="AF82" s="28"/>
+      <c r="AG82" s="28"/>
+    </row>
+    <row r="83" spans="2:33" ht="10" customHeight="1">
+      <c r="AF83" s="28"/>
+      <c r="AG83" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>